<commit_message>
saved updates in excel
</commit_message>
<xml_diff>
--- a/PracticeList.xlsx
+++ b/PracticeList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lxie1/personal/codingpractice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A75CCB3-9507-5C45-AB74-E7D62CCA362C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7BF65CC-EB59-4048-A564-3C1B13782B97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="820" windowWidth="35840" windowHeight="20200" activeTab="10" xr2:uid="{7D075F38-A8A9-0349-9089-EC4AFD30F784}"/>
+    <workbookView xWindow="0" yWindow="820" windowWidth="35840" windowHeight="20200" xr2:uid="{7D075F38-A8A9-0349-9089-EC4AFD30F784}"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
@@ -2819,6 +2819,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2872,9 +2875,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3193,7 +3193,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C4AC671-66B9-9043-8EF5-2D6A00DBDF6A}">
   <dimension ref="A1:T64"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="108" zoomScaleNormal="109" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="108" zoomScaleNormal="109" workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -4599,13 +4599,13 @@
       <c r="B1" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="C1" s="218" t="s">
+      <c r="C1" s="219" t="s">
         <v>103</v>
       </c>
-      <c r="D1" s="218"/>
-      <c r="E1" s="218"/>
-      <c r="F1" s="218"/>
-      <c r="G1" s="219"/>
+      <c r="D1" s="219"/>
+      <c r="E1" s="219"/>
+      <c r="F1" s="219"/>
+      <c r="G1" s="220"/>
       <c r="H1" s="14" t="s">
         <v>104</v>
       </c>
@@ -4721,7 +4721,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E27620F9-994B-C149-BBC2-5A7647DF3CE9}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
+    <sheetView zoomScale="101" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -4745,13 +4745,13 @@
       <c r="B1" s="81" t="s">
         <v>102</v>
       </c>
-      <c r="C1" s="229" t="s">
+      <c r="C1" s="230" t="s">
         <v>103</v>
       </c>
-      <c r="D1" s="229"/>
-      <c r="E1" s="229"/>
-      <c r="F1" s="229"/>
-      <c r="G1" s="230"/>
+      <c r="D1" s="230"/>
+      <c r="E1" s="230"/>
+      <c r="F1" s="230"/>
+      <c r="G1" s="231"/>
       <c r="H1" s="82" t="s">
         <v>104</v>
       </c>
@@ -4925,7 +4925,7 @@
     </row>
     <row r="12" spans="1:8" ht="17" thickBot="1">
       <c r="A12" s="100"/>
-      <c r="B12" s="235"/>
+      <c r="B12" s="217"/>
       <c r="C12" s="102"/>
       <c r="D12" s="102"/>
       <c r="E12" s="102"/>
@@ -4998,13 +4998,13 @@
       <c r="B1" s="184" t="s">
         <v>102</v>
       </c>
-      <c r="C1" s="232" t="s">
+      <c r="C1" s="233" t="s">
         <v>103</v>
       </c>
-      <c r="D1" s="220"/>
-      <c r="E1" s="220"/>
-      <c r="F1" s="220"/>
-      <c r="G1" s="220"/>
+      <c r="D1" s="221"/>
+      <c r="E1" s="221"/>
+      <c r="F1" s="221"/>
+      <c r="G1" s="221"/>
       <c r="J1" s="152"/>
       <c r="K1" s="130" t="s">
         <v>104</v>
@@ -5356,14 +5356,14 @@
       <c r="B1" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="C1" s="217" t="s">
+      <c r="C1" s="218" t="s">
         <v>103</v>
       </c>
-      <c r="D1" s="218"/>
-      <c r="E1" s="218"/>
-      <c r="F1" s="218"/>
-      <c r="G1" s="218"/>
-      <c r="H1" s="218"/>
+      <c r="D1" s="219"/>
+      <c r="E1" s="219"/>
+      <c r="F1" s="219"/>
+      <c r="G1" s="219"/>
+      <c r="H1" s="219"/>
       <c r="I1" s="120"/>
       <c r="J1" s="121"/>
       <c r="K1" s="14" t="s">
@@ -5645,13 +5645,13 @@
       <c r="B1" s="128" t="s">
         <v>102</v>
       </c>
-      <c r="C1" s="233" t="s">
+      <c r="C1" s="234" t="s">
         <v>103</v>
       </c>
-      <c r="D1" s="220"/>
-      <c r="E1" s="220"/>
-      <c r="F1" s="220"/>
-      <c r="G1" s="221"/>
+      <c r="D1" s="221"/>
+      <c r="E1" s="221"/>
+      <c r="F1" s="221"/>
+      <c r="G1" s="222"/>
       <c r="H1" s="130" t="s">
         <v>104</v>
       </c>
@@ -5886,14 +5886,14 @@
       <c r="B1" s="129" t="s">
         <v>102</v>
       </c>
-      <c r="C1" s="220" t="s">
+      <c r="C1" s="221" t="s">
         <v>103</v>
       </c>
-      <c r="D1" s="234"/>
-      <c r="E1" s="220"/>
-      <c r="F1" s="220"/>
-      <c r="G1" s="220"/>
-      <c r="H1" s="221"/>
+      <c r="D1" s="235"/>
+      <c r="E1" s="221"/>
+      <c r="F1" s="221"/>
+      <c r="G1" s="221"/>
+      <c r="H1" s="222"/>
       <c r="I1" s="130" t="s">
         <v>104</v>
       </c>
@@ -6278,13 +6278,13 @@
       <c r="B1" s="81" t="s">
         <v>102</v>
       </c>
-      <c r="C1" s="229" t="s">
+      <c r="C1" s="230" t="s">
         <v>103</v>
       </c>
-      <c r="D1" s="229"/>
-      <c r="E1" s="229"/>
-      <c r="F1" s="229"/>
-      <c r="G1" s="230"/>
+      <c r="D1" s="230"/>
+      <c r="E1" s="230"/>
+      <c r="F1" s="230"/>
+      <c r="G1" s="231"/>
       <c r="H1" s="82" t="s">
         <v>104</v>
       </c>
@@ -6486,13 +6486,13 @@
       <c r="B1" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="C1" s="217" t="s">
+      <c r="C1" s="218" t="s">
         <v>103</v>
       </c>
-      <c r="D1" s="218"/>
-      <c r="E1" s="218"/>
-      <c r="F1" s="218"/>
-      <c r="G1" s="219"/>
+      <c r="D1" s="219"/>
+      <c r="E1" s="219"/>
+      <c r="F1" s="219"/>
+      <c r="G1" s="220"/>
       <c r="H1" s="14" t="s">
         <v>104</v>
       </c>
@@ -6633,13 +6633,13 @@
       <c r="B1" s="127" t="s">
         <v>102</v>
       </c>
-      <c r="C1" s="220" t="s">
+      <c r="C1" s="221" t="s">
         <v>103</v>
       </c>
-      <c r="D1" s="220"/>
-      <c r="E1" s="220"/>
-      <c r="F1" s="220"/>
-      <c r="G1" s="221"/>
+      <c r="D1" s="221"/>
+      <c r="E1" s="221"/>
+      <c r="F1" s="221"/>
+      <c r="G1" s="222"/>
       <c r="H1" s="130" t="s">
         <v>104</v>
       </c>
@@ -6778,13 +6778,13 @@
       <c r="B1" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="C1" s="222" t="s">
+      <c r="C1" s="223" t="s">
         <v>103</v>
       </c>
-      <c r="D1" s="222"/>
-      <c r="E1" s="222"/>
-      <c r="F1" s="222"/>
-      <c r="G1" s="222"/>
+      <c r="D1" s="223"/>
+      <c r="E1" s="223"/>
+      <c r="F1" s="223"/>
+      <c r="G1" s="223"/>
       <c r="H1" s="38"/>
       <c r="I1" s="38"/>
       <c r="J1" s="39"/>
@@ -6953,19 +6953,19 @@
       <c r="K11" s="40"/>
     </row>
     <row r="15" spans="1:11">
-      <c r="A15" s="223" t="s">
+      <c r="A15" s="224" t="s">
         <v>211</v>
       </c>
-      <c r="B15" s="224"/>
-      <c r="C15" s="224"/>
-      <c r="D15" s="224"/>
-      <c r="E15" s="224"/>
-      <c r="F15" s="224"/>
-      <c r="G15" s="224"/>
-      <c r="H15" s="224"/>
-      <c r="I15" s="224"/>
-      <c r="J15" s="224"/>
-      <c r="K15" s="224"/>
+      <c r="B15" s="225"/>
+      <c r="C15" s="225"/>
+      <c r="D15" s="225"/>
+      <c r="E15" s="225"/>
+      <c r="F15" s="225"/>
+      <c r="G15" s="225"/>
+      <c r="H15" s="225"/>
+      <c r="I15" s="225"/>
+      <c r="J15" s="225"/>
+      <c r="K15" s="225"/>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="29" t="s">
@@ -7035,13 +7035,13 @@
       <c r="B1" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="C1" s="225" t="s">
+      <c r="C1" s="226" t="s">
         <v>103</v>
       </c>
-      <c r="D1" s="222"/>
-      <c r="E1" s="222"/>
-      <c r="F1" s="222"/>
-      <c r="G1" s="222"/>
+      <c r="D1" s="223"/>
+      <c r="E1" s="223"/>
+      <c r="F1" s="223"/>
+      <c r="G1" s="223"/>
       <c r="H1" s="38"/>
       <c r="I1" s="39"/>
       <c r="J1" s="28" t="s">
@@ -7247,13 +7247,13 @@
       <c r="B1" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="C1" s="217" t="s">
+      <c r="C1" s="218" t="s">
         <v>103</v>
       </c>
-      <c r="D1" s="218"/>
-      <c r="E1" s="226"/>
-      <c r="F1" s="218"/>
-      <c r="G1" s="219"/>
+      <c r="D1" s="219"/>
+      <c r="E1" s="227"/>
+      <c r="F1" s="219"/>
+      <c r="G1" s="220"/>
       <c r="H1" s="14" t="s">
         <v>104</v>
       </c>
@@ -7406,14 +7406,14 @@
       <c r="B1" s="53" t="s">
         <v>102</v>
       </c>
-      <c r="C1" s="227" t="s">
+      <c r="C1" s="228" t="s">
         <v>103</v>
       </c>
-      <c r="D1" s="228"/>
-      <c r="E1" s="228"/>
-      <c r="F1" s="228"/>
-      <c r="G1" s="228"/>
-      <c r="H1" s="228"/>
+      <c r="D1" s="229"/>
+      <c r="E1" s="229"/>
+      <c r="F1" s="229"/>
+      <c r="G1" s="229"/>
+      <c r="H1" s="229"/>
       <c r="I1" s="67"/>
       <c r="J1" s="67"/>
       <c r="K1" s="54" t="s">
@@ -7688,13 +7688,13 @@
       <c r="B1" s="81" t="s">
         <v>102</v>
       </c>
-      <c r="C1" s="229" t="s">
+      <c r="C1" s="230" t="s">
         <v>103</v>
       </c>
-      <c r="D1" s="229"/>
-      <c r="E1" s="229"/>
-      <c r="F1" s="229"/>
-      <c r="G1" s="230"/>
+      <c r="D1" s="230"/>
+      <c r="E1" s="230"/>
+      <c r="F1" s="230"/>
+      <c r="G1" s="231"/>
       <c r="H1" s="82" t="s">
         <v>104</v>
       </c>
@@ -7843,13 +7843,13 @@
       <c r="B1" s="156" t="s">
         <v>102</v>
       </c>
-      <c r="C1" s="231" t="s">
+      <c r="C1" s="232" t="s">
         <v>103</v>
       </c>
-      <c r="D1" s="231"/>
-      <c r="E1" s="231"/>
-      <c r="F1" s="231"/>
-      <c r="G1" s="231"/>
+      <c r="D1" s="232"/>
+      <c r="E1" s="232"/>
+      <c r="F1" s="232"/>
+      <c r="G1" s="232"/>
       <c r="H1" s="157"/>
       <c r="I1" s="158"/>
       <c r="J1" s="159" t="s">

</xml_diff>